<commit_message>
Integrated Excel capabilites to the framework
</commit_message>
<xml_diff>
--- a/data/SeleniumLogin.xlsx
+++ b/data/SeleniumLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karthick\GitProjects\Selenium_Framework_2.0\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07FDAF-B092-4A47-9E53-736CF518D1F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21411656-1F14-49BA-9A7D-4F0F7AA32C1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>admin</t>
   </si>
@@ -34,16 +34,40 @@
   </si>
   <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>stestcasename</t>
+  </si>
+  <si>
+    <t>AmazonLoginPageTest</t>
+  </si>
+  <si>
+    <t>admin@abc.com</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>OrangeHRMLoginTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,66 +376,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>